<commit_message>
HW3 Addednum for 64 Core Machine
</commit_message>
<xml_diff>
--- a/HW3_Addendum.xlsx
+++ b/HW3_Addendum.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="14320" yWindow="0" windowWidth="14400" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,20 +36,20 @@
     <t>All CPUs</t>
   </si>
   <si>
-    <t>Less than 1 CPU</t>
-  </si>
-  <si>
     <t>Two CPUs</t>
   </si>
   <si>
     <t>Three CPUs</t>
+  </si>
+  <si>
+    <t>&lt; 1 CPU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,8 +79,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,24 +96,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7C702"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,7 +263,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,8 +279,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -318,7 +308,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -340,13 +329,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -361,29 +343,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -391,6 +353,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -398,6 +361,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,11 +532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143185224"/>
-        <c:axId val="-2143176536"/>
+        <c:axId val="303510760"/>
+        <c:axId val="303517736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143185224"/>
+        <c:axId val="303510760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,14 +549,14 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
                   <a:t> of Threads</a:t>
                 </a:r>
               </a:p>
@@ -604,7 +568,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143176536"/>
+        <c:crossAx val="303517736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -612,7 +576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143176536"/>
+        <c:axId val="303517736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,10 +590,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Operations</a:t>
                 </a:r>
               </a:p>
@@ -642,7 +606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143185224"/>
+        <c:crossAx val="303510760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -657,6 +621,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -833,11 +807,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141667544"/>
-        <c:axId val="-2139972504"/>
+        <c:axId val="114263224"/>
+        <c:axId val="114268792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141667544"/>
+        <c:axId val="114263224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,14 +824,14 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
                   <a:t> of Threads</a:t>
                 </a:r>
               </a:p>
@@ -869,7 +843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139972504"/>
+        <c:crossAx val="114268792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -877,7 +851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2139972504"/>
+        <c:axId val="114268792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,10 +865,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Operations</a:t>
                 </a:r>
               </a:p>
@@ -907,7 +881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141667544"/>
+        <c:crossAx val="114263224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -922,6 +896,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -946,9 +930,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1193800</xdr:colOff>
+      <xdr:colOff>1460500</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -976,9 +960,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1326,19 +1310,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20" thickTop="1" thickBot="1">
@@ -1388,25 +1372,25 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="31">
+      <c r="A3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="18">
         <v>2</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="19">
         <v>2521000</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="18">
         <v>2</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="19">
         <v>2665000</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="18">
         <v>2</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="19">
         <v>5043000</v>
       </c>
       <c r="H3" s="3"/>
@@ -1415,23 +1399,23 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="18">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18">
         <v>4</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="19">
         <v>1553000</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="18">
         <v>4</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="19">
         <v>2210500</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="18">
         <v>4</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="19">
         <v>4514500</v>
       </c>
       <c r="H4" s="3"/>
@@ -1440,23 +1424,23 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="18">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18">
         <v>8</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="19">
         <v>1239000</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="18">
         <v>8</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="19">
         <v>1444500</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="18">
         <v>8</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="19">
         <v>4447500</v>
       </c>
       <c r="H5" s="3"/>
@@ -1465,23 +1449,23 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="18">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18">
         <v>12</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="19">
         <v>1606500</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="18">
         <v>12</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="19">
         <v>1343000</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="18">
         <v>12</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="19">
         <v>3160000</v>
       </c>
       <c r="H6" s="3"/>
@@ -1490,23 +1474,23 @@
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="18">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18">
         <v>16</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="19">
         <v>1597000</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="18">
         <v>16</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="19">
         <v>1393500</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="18">
         <v>16</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="19">
         <v>3060500</v>
       </c>
       <c r="H7" s="3"/>
@@ -1515,25 +1499,25 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="18">
-      <c r="A8" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="28">
+      <c r="A8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="21">
         <v>24</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="22">
         <v>1372500</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="21">
         <v>24</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="22">
         <v>1656000</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="21">
         <v>24</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="22">
         <v>2800000</v>
       </c>
       <c r="H8" s="3"/>
@@ -1542,23 +1526,23 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="18">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21">
         <v>32</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="22">
         <v>1437500</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="21">
         <v>32</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="22">
         <v>1312000</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="21">
         <v>32</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="22">
         <v>2694500</v>
       </c>
       <c r="H9" s="3"/>
@@ -1567,25 +1551,25 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="18">
-      <c r="A10" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="25">
+      <c r="A10" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="24">
         <v>40</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="25">
         <v>1293000</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>40</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <v>1567000</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>40</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <v>2566000</v>
       </c>
       <c r="H10" s="3"/>
@@ -1594,23 +1578,23 @@
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="18">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="24">
         <v>48</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>1311500</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>48</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <v>1294500</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>48</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <v>2558500</v>
       </c>
       <c r="H11" s="3"/>
@@ -1619,25 +1603,25 @@
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="18">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="12">
         <v>56</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="13">
         <v>1212000</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="12">
         <v>56</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="13">
         <v>1348500</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="12">
         <v>56</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="13">
         <v>2344000</v>
       </c>
       <c r="H12" s="3"/>
@@ -1646,23 +1630,23 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="19" thickBot="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15">
         <v>64</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="16">
         <v>1243000</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="15">
         <v>64</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="16">
         <v>1335500</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="15">
         <v>64</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="16">
         <v>2333500</v>
       </c>
       <c r="H13" s="3"/>
@@ -1736,25 +1720,25 @@
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="18">
-      <c r="A18" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="31">
+      <c r="A18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="18">
         <v>2</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="19">
         <v>2462949</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="18">
         <v>2</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="19">
         <v>2053159</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="18">
         <v>2</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="19">
         <v>1466438</v>
       </c>
       <c r="H18" s="3"/>
@@ -1763,23 +1747,23 @@
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" ht="18">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18">
         <v>4</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="19">
         <v>3197000</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="18">
         <v>4</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="19">
         <v>5041500</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="18">
         <v>4</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="19">
         <v>2027273</v>
       </c>
       <c r="H19" s="3"/>
@@ -1788,125 +1772,125 @@
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="18">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18">
         <v>8</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="19">
         <v>1055381</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="18">
         <v>8</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="19">
         <v>1647170</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="18">
         <v>8</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="19">
         <v>2190711</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18">
         <v>12</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="19">
         <v>500946</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="18">
         <v>12</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="19">
         <v>565433</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="18">
         <v>12</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="19">
         <v>2007097</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18">
         <v>16</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="19">
         <v>110815</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="18">
         <v>16</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="19">
         <v>358420</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="18">
         <v>16</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="19">
         <v>2114130</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1">
-      <c r="A23" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="34">
+      <c r="A23" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="21">
         <v>24</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="22">
         <v>1297500</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="21">
         <v>24</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="22">
         <v>2234000</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="21">
         <v>24</v>
       </c>
-      <c r="G23" s="35">
+      <c r="G23" s="22">
         <v>1118682</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
     </row>
     <row r="24" spans="1:11" ht="18">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21">
         <v>32</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="22">
         <v>1362163</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="21">
         <v>32</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="22">
         <v>2539500</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="21">
         <v>32</v>
       </c>
-      <c r="G24" s="35">
+      <c r="G24" s="22">
         <v>1337761</v>
       </c>
       <c r="H24" s="3"/>
@@ -1915,25 +1899,25 @@
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="18">
-      <c r="A25" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="37">
+      <c r="A25" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="24">
         <v>40</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="25">
         <v>812000</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="24">
         <v>40</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="25">
         <v>1065034</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="24">
         <v>40</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="25">
         <v>1052817</v>
       </c>
       <c r="H25" s="3"/>
@@ -1942,23 +1926,23 @@
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" ht="18">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37">
+      <c r="A26" s="23"/>
+      <c r="B26" s="24">
         <v>48</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C26" s="25">
         <v>712279</v>
       </c>
-      <c r="D26" s="37">
+      <c r="D26" s="24">
         <v>48</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E26" s="25">
         <v>728908</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="24">
         <v>48</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="25">
         <v>1038676</v>
       </c>
       <c r="H26" s="3"/>
@@ -1967,25 +1951,25 @@
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" ht="18">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="12">
         <v>56</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="13">
         <v>617000</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="12">
         <v>56</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="13">
         <v>815232</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="12">
         <v>56</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>964756</v>
       </c>
       <c r="H27" s="3"/>
@@ -1994,23 +1978,23 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" ht="19" thickBot="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15">
         <v>64</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="16">
         <v>632000</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="15">
         <v>64</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="16">
         <v>283226</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <v>64</v>
       </c>
-      <c r="G28" s="17">
+      <c r="G28" s="16">
         <v>378500</v>
       </c>
       <c r="H28" s="3"/>
@@ -2274,6 +2258,7 @@
     <mergeCell ref="J20:J23"/>
     <mergeCell ref="K20:K23"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>